<commit_message>
finaliza jornada QH 21-11-2014
</commit_message>
<xml_diff>
--- a/Documentacion/estructuras-informacion.xlsx
+++ b/Documentacion/estructuras-informacion.xlsx
@@ -13,7 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Correlativas" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="acuerdos" sheetId="2" r:id="rId2"/>
+    <sheet name="tipo_contingente" sheetId="4" r:id="rId3"/>
+    <sheet name="tipo_desgravacion" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>posición arancelaria origen</t>
   </si>
@@ -33,9 +35,6 @@
     <t>posición arancelaria destino</t>
   </si>
   <si>
-    <t>Fecha en que entra en vigencia el cambio (AAAA-mm)</t>
-  </si>
-  <si>
     <t>Número del decreto</t>
   </si>
   <si>
@@ -45,9 +44,6 @@
     <t>Estructura para las Correlativas</t>
   </si>
   <si>
-    <t>Texto de 10</t>
-  </si>
-  <si>
     <t>Campo</t>
   </si>
   <si>
@@ -61,6 +57,135 @@
   </si>
   <si>
     <t>Texto largo</t>
+  </si>
+  <si>
+    <t>Fecha en que entra en vigencia el cambio (AAAA-mm-dd)</t>
+  </si>
+  <si>
+    <t>contingente</t>
+  </si>
+  <si>
+    <t>arancel %</t>
+  </si>
+  <si>
+    <t>salvador</t>
+  </si>
+  <si>
+    <t>año</t>
+  </si>
+  <si>
+    <t>contingente Tn</t>
+  </si>
+  <si>
+    <t>acuerdo</t>
+  </si>
+  <si>
+    <t>tipo_contingente_id</t>
+  </si>
+  <si>
+    <t>tipo_contingente_nombre</t>
+  </si>
+  <si>
+    <t>no tiene limite de peso</t>
+  </si>
+  <si>
+    <t>tipo_contingente_mlimite</t>
+  </si>
+  <si>
+    <t>tipo_contingente_mmultiano</t>
+  </si>
+  <si>
+    <t>los productos para este contingente tiene limite de peso? Podrian no manejar limite de peso como el acuerdo con el salvador para la posicion 2309.10.90.00</t>
+  </si>
+  <si>
+    <t>si maneja limite de peso se debe preguntar si este limite varia con los años o es el mismo para todos los años del acuerdo</t>
+  </si>
+  <si>
+    <t>se debe preguntar si las cantidades son acumuladas para los paises con los que establece el acuerdo o se manejan individual para cada pais</t>
+  </si>
+  <si>
+    <t>limite gradual</t>
+  </si>
+  <si>
+    <t>limite fijo</t>
+  </si>
+  <si>
+    <t>lmite gradual multipais</t>
+  </si>
+  <si>
+    <t>tipo_contingente_mmultipais</t>
+  </si>
+  <si>
+    <t>contingente_det_id</t>
+  </si>
+  <si>
+    <t>contingente_det_periodo</t>
+  </si>
+  <si>
+    <t>acuerdo_det</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_acuerdo_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_posiciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_arancel_base </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_tipo_contingente_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_tipo_desgravacion_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_nperiodos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_msalvaguardia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_det_administracion </t>
+  </si>
+  <si>
+    <t>acuerdo_det_administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_nombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_descripcion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_intercambio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_paises </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_fvigente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_uinsert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_finsert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acuerdo_uupdate </t>
+  </si>
+  <si>
+    <t>acuerdo_fupdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -92,7 +217,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -174,19 +299,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -220,26 +332,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +641,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,57 +654,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -600,9 +718,468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <v>2010</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6">
+        <v>2011</v>
+      </c>
+      <c r="J6">
+        <v>-1</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7">
+        <v>2012</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="12">
+        <f>K6-4%</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>2013</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" ref="K8:K14" si="0">K7-4%</f>
+        <v>0.24000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9">
+        <v>2014</v>
+      </c>
+      <c r="J9">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>2015</v>
+      </c>
+      <c r="J10">
+        <v>-1</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11">
+        <v>2016</v>
+      </c>
+      <c r="J11">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
+        <v>2017</v>
+      </c>
+      <c r="J12">
+        <v>-1</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="0"/>
+        <v>7.9999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2018</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="0"/>
+        <v>3.9999999999999987E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>2019</v>
+      </c>
+      <c r="J14">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>2020</v>
+      </c>
+      <c r="J15">
+        <v>-1</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2021</v>
+      </c>
+      <c r="J16">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>